<commit_message>
Add support for analytic tags
Move all speeddicts to dedicated prepare method
XLSX import : fix bug when debit/credit is an integer
Improve multi-company support
</commit_message>
<xml_diff>
--- a/account_move_csv_import/demo/account_move_generic-fr_coa.xlsx
+++ b/account_move_csv_import/demo/account_move_generic-fr_coa.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t xml:space="preserve">MISC</t>
   </si>
@@ -34,7 +34,16 @@
     <t xml:space="preserve">PUR</t>
   </si>
   <si>
+    <t xml:space="preserve">CONTRACTS,B2B</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUPP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2B, B2C,</t>
   </si>
   <si>
     <t xml:space="preserve">Caution locaux</t>
@@ -59,6 +68,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,19 +154,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.73"/>
@@ -221,6 +231,9 @@
       <c r="H3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="K3" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -233,7 +246,7 @@
         <v>641300</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>1</v>
@@ -244,6 +257,9 @@
       <c r="H4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="K4" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -267,6 +283,9 @@
       <c r="H5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="K5" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -279,13 +298,13 @@
         <v>275100</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1642.42</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,13 +318,13 @@
         <v>512001</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>1642.42</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,7 +338,7 @@
         <v>421000</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>12042.12</v>
@@ -339,7 +358,7 @@
         <v>512001</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>12042.12</v>

</xml_diff>

<commit_message>
[MIG] account_move_csv_import from v14 to v16
</commit_message>
<xml_diff>
--- a/account_move_csv_import/demo/account_move_generic-fr_coa.xlsx
+++ b/account_move_csv_import/demo/account_move_generic-fr_coa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t xml:space="preserve">MISC</t>
   </si>
@@ -34,16 +34,10 @@
     <t xml:space="preserve">PUR</t>
   </si>
   <si>
-    <t xml:space="preserve">CONTRACTS,B2B</t>
-  </si>
-  <si>
     <t xml:space="preserve">SUPP</t>
   </si>
   <si>
-    <t xml:space="preserve">B2G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B2B, B2C,</t>
+    <t xml:space="preserve">PUR : 35 | SUPP : 65</t>
   </si>
   <si>
     <t xml:space="preserve">Caution locaux</t>
@@ -154,19 +148,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.73"/>
@@ -231,9 +225,6 @@
       <c r="H3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -246,7 +237,7 @@
         <v>641300</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>1</v>
@@ -257,9 +248,6 @@
       <c r="H4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -272,7 +260,7 @@
         <v>645100</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>1</v>
@@ -283,9 +271,6 @@
       <c r="H5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -298,13 +283,13 @@
         <v>275100</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1642.42</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,13 +303,13 @@
         <v>512001</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>1642.42</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -338,7 +323,7 @@
         <v>421000</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>12042.12</v>
@@ -358,7 +343,7 @@
         <v>512001</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>12042.12</v>

</xml_diff>

<commit_message>
Add support for generic XLS and ODS files
</commit_message>
<xml_diff>
--- a/account_move_csv_import/demo/account_move_generic-fr_coa.xlsx
+++ b/account_move_csv_import/demo/account_move_generic-fr_coa.xlsx
@@ -151,10 +151,10 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.16"/>

</xml_diff>